<commit_message>
C# Day 4 Documents
</commit_message>
<xml_diff>
--- a/Fundamental_Primer_Program_Phase1.xlsx
+++ b/Fundamental_Primer_Program_Phase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anami\Wipro_24thJune\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712D30A8-18C3-4870-BBBF-3789A84C677B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCBB4E1-221C-48C8-BA19-0D4EBB8A90D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -985,7 +985,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1020,18 +1020,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1074,6 +1068,36 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1136,24 +1160,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1448,55 +1454,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <f>SUM(B3:B6)</f>
         <v>10</v>
       </c>
@@ -1514,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874799AA-154E-41D6-97CF-30639D88BFCA}">
   <dimension ref="A1:E197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1545,357 +1551,357 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="37">
+      <c r="A3" s="45">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="35"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="38"/>
-      <c r="B4" s="54" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="38"/>
-      <c r="B5" s="54" t="s">
+      <c r="A5" s="46"/>
+      <c r="B5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="43"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="38"/>
-      <c r="B6" s="54" t="s">
+      <c r="A6" s="46"/>
+      <c r="B6" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="35"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="43"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="38"/>
-      <c r="B7" s="54" t="s">
+      <c r="A7" s="46"/>
+      <c r="B7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="35"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="38"/>
-      <c r="B8" s="54" t="s">
+      <c r="A8" s="46"/>
+      <c r="B8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="35"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="43"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="39"/>
-      <c r="B9" s="54" t="s">
+      <c r="A9" s="47"/>
+      <c r="B9" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="35"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="43"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="37">
+      <c r="A10" s="45">
         <v>1.2</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="35"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="43"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="38"/>
-      <c r="B11" s="54" t="s">
+      <c r="A11" s="46"/>
+      <c r="B11" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="35"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="43"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="38"/>
-      <c r="B12" s="54" t="s">
+      <c r="A12" s="46"/>
+      <c r="B12" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="35"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="43"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="39"/>
-      <c r="B13" s="54" t="s">
+      <c r="A13" s="47"/>
+      <c r="B13" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="35"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="43"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="37">
+      <c r="A14" s="45">
         <v>1.3</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="35"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="43"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="38"/>
-      <c r="B15" s="56" t="s">
+      <c r="A15" s="46"/>
+      <c r="B15" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="35"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="43"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="38"/>
-      <c r="B16" s="56" t="s">
+      <c r="A16" s="46"/>
+      <c r="B16" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="35"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="43"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="37">
+      <c r="A17" s="45">
         <v>1.4</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="35"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="43"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="38"/>
-      <c r="B18" s="24" t="s">
+      <c r="A18" s="46"/>
+      <c r="B18" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="35"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="43"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="38"/>
-      <c r="B19" s="24" t="s">
+      <c r="A19" s="46"/>
+      <c r="B19" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="35"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="43"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="39"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="47"/>
+      <c r="B20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="35"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="43"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="37">
+      <c r="A21" s="45">
         <v>1.5</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="35"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="43"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="38"/>
-      <c r="B22" s="54" t="s">
+      <c r="A22" s="46"/>
+      <c r="B22" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="35"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="43"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="38"/>
-      <c r="B23" s="54" t="s">
+      <c r="A23" s="46"/>
+      <c r="B23" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="35"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="43"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="39"/>
-      <c r="B24" s="54" t="s">
+      <c r="A24" s="47"/>
+      <c r="B24" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="36"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="44"/>
     </row>
     <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>2</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="48" t="s">
         <v>211</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D25" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="50" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="37">
+      <c r="A26" s="45">
         <v>2.1</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="42"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="50"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="38"/>
-      <c r="B27" s="25" t="s">
+      <c r="A27" s="46"/>
+      <c r="B27" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="42"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="50"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="38"/>
-      <c r="B28" s="25" t="s">
+      <c r="A28" s="46"/>
+      <c r="B28" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="42"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="50"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="39"/>
-      <c r="B29" s="25" t="s">
+      <c r="A29" s="47"/>
+      <c r="B29" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="42"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="50"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="37">
+      <c r="A30" s="45">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="50"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="38"/>
-      <c r="B31" s="25" t="s">
+      <c r="A31" s="46"/>
+      <c r="B31" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="42"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="50"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="38"/>
-      <c r="B32" s="25" t="s">
+      <c r="A32" s="46"/>
+      <c r="B32" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="50"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="39"/>
-      <c r="B33" s="25" t="s">
+      <c r="A33" s="47"/>
+      <c r="B33" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="42"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="50"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="37">
+      <c r="A34" s="45">
         <v>2.6</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="42"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="38"/>
-      <c r="B35" s="25" t="s">
+      <c r="A35" s="46"/>
+      <c r="B35" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="42"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="38"/>
-      <c r="B36" s="25" t="s">
+      <c r="A36" s="46"/>
+      <c r="B36" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="42"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="50"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="39"/>
-      <c r="B37" s="25" t="s">
+      <c r="A37" s="47"/>
+      <c r="B37" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="42"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="50"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="7"/>
@@ -1922,394 +1928,394 @@
       <c r="B40" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="45">
+      <c r="D40" s="53">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="46">
+      <c r="A41" s="54">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B41" s="51" t="s">
+      <c r="B41" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="44"/>
-      <c r="D41" s="45"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="53"/>
     </row>
     <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="46"/>
-      <c r="B42" s="52" t="s">
+      <c r="A42" s="54"/>
+      <c r="B42" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="45"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="53"/>
     </row>
     <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="46"/>
-      <c r="B43" s="52" t="s">
+      <c r="A43" s="54"/>
+      <c r="B43" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="45"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="53"/>
     </row>
     <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="46"/>
-      <c r="B44" s="52" t="s">
+      <c r="A44" s="54"/>
+      <c r="B44" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="45"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
     </row>
     <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="46">
+      <c r="A45" s="54">
         <v>1.2</v>
       </c>
-      <c r="B45" s="51" t="s">
+      <c r="B45" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="45"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="53"/>
     </row>
     <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="46"/>
-      <c r="B46" s="52" t="s">
+      <c r="A46" s="54"/>
+      <c r="B46" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="45"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="53"/>
     </row>
     <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="46"/>
-      <c r="B47" s="52" t="s">
+      <c r="A47" s="54"/>
+      <c r="B47" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="45"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="53"/>
     </row>
     <row r="48" spans="1:5" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="46">
+      <c r="A48" s="54">
         <v>1.3</v>
       </c>
-      <c r="B48" s="51" t="s">
+      <c r="B48" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="45"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="53"/>
     </row>
     <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="46"/>
-      <c r="B49" s="52" t="s">
+      <c r="A49" s="54"/>
+      <c r="B49" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="44"/>
-      <c r="D49" s="45"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="53"/>
     </row>
     <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="46"/>
-      <c r="B50" s="52" t="s">
+      <c r="A50" s="54"/>
+      <c r="B50" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="44"/>
-      <c r="D50" s="45"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="53"/>
     </row>
     <row r="51" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="46"/>
-      <c r="B51" s="52" t="s">
+      <c r="A51" s="54"/>
+      <c r="B51" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="44"/>
-      <c r="D51" s="45"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="53"/>
     </row>
     <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="46">
+      <c r="A52" s="54">
         <v>1.4</v>
       </c>
-      <c r="B52" s="51" t="s">
+      <c r="B52" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="45"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="53"/>
     </row>
     <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="46"/>
-      <c r="B53" s="52" t="s">
+      <c r="A53" s="54"/>
+      <c r="B53" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C53" s="44"/>
-      <c r="D53" s="45"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="53"/>
     </row>
     <row r="54" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="46"/>
-      <c r="B54" s="52" t="s">
+      <c r="A54" s="54"/>
+      <c r="B54" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="44"/>
-      <c r="D54" s="45"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="53"/>
     </row>
     <row r="55" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="46">
+      <c r="A55" s="54">
         <v>1.5</v>
       </c>
-      <c r="B55" s="51" t="s">
+      <c r="B55" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="44"/>
-      <c r="D55" s="45"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="53"/>
     </row>
     <row r="56" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="46"/>
-      <c r="B56" s="52" t="s">
+      <c r="A56" s="54"/>
+      <c r="B56" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C56" s="44"/>
-      <c r="D56" s="45"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="53"/>
     </row>
     <row r="57" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="46"/>
-      <c r="B57" s="52" t="s">
+      <c r="A57" s="54"/>
+      <c r="B57" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C57" s="44"/>
-      <c r="D57" s="45"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="53"/>
     </row>
     <row r="58" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3">
         <v>2</v>
       </c>
-      <c r="B58" s="53" t="s">
+      <c r="B58" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="44"/>
-      <c r="D58" s="45"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="53"/>
     </row>
     <row r="59" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="46">
+      <c r="A59" s="54">
         <v>2.1</v>
       </c>
-      <c r="B59" s="51" t="s">
+      <c r="B59" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="44"/>
-      <c r="D59" s="45"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="53"/>
     </row>
     <row r="60" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="46"/>
-      <c r="B60" s="52" t="s">
+      <c r="A60" s="54"/>
+      <c r="B60" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C60" s="44"/>
-      <c r="D60" s="45"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="53"/>
     </row>
     <row r="61" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="46"/>
-      <c r="B61" s="52" t="s">
+      <c r="A61" s="54"/>
+      <c r="B61" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C61" s="44"/>
-      <c r="D61" s="45"/>
+      <c r="C61" s="52"/>
+      <c r="D61" s="53"/>
     </row>
     <row r="62" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="43">
+      <c r="A62" s="51">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B62" s="51" t="s">
+      <c r="B62" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="44"/>
-      <c r="D62" s="45"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="53"/>
     </row>
     <row r="63" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="43"/>
-      <c r="B63" s="52" t="s">
+      <c r="A63" s="51"/>
+      <c r="B63" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C63" s="44"/>
-      <c r="D63" s="45"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="53"/>
     </row>
     <row r="64" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="43"/>
-      <c r="B64" s="52" t="s">
+      <c r="A64" s="51"/>
+      <c r="B64" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C64" s="44"/>
-      <c r="D64" s="45"/>
+      <c r="C64" s="52"/>
+      <c r="D64" s="53"/>
     </row>
     <row r="65" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="43"/>
-      <c r="B65" s="52" t="s">
+      <c r="A65" s="51"/>
+      <c r="B65" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="44"/>
-      <c r="D65" s="45"/>
+      <c r="C65" s="52"/>
+      <c r="D65" s="53"/>
     </row>
     <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="43">
+      <c r="A66" s="51">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B66" s="51" t="s">
+      <c r="B66" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C66" s="44"/>
-      <c r="D66" s="45"/>
+      <c r="C66" s="52"/>
+      <c r="D66" s="53"/>
     </row>
     <row r="67" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="43"/>
-      <c r="B67" s="52" t="s">
+      <c r="A67" s="51"/>
+      <c r="B67" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C67" s="44"/>
-      <c r="D67" s="45"/>
+      <c r="C67" s="52"/>
+      <c r="D67" s="53"/>
     </row>
     <row r="68" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="43"/>
-      <c r="B68" s="52" t="s">
+      <c r="A68" s="51"/>
+      <c r="B68" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C68" s="44"/>
-      <c r="D68" s="45"/>
+      <c r="C68" s="52"/>
+      <c r="D68" s="53"/>
     </row>
     <row r="69" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="43">
+      <c r="A69" s="51">
         <v>2.4</v>
       </c>
-      <c r="B69" s="51" t="s">
+      <c r="B69" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C69" s="44"/>
-      <c r="D69" s="45"/>
+      <c r="C69" s="52"/>
+      <c r="D69" s="53"/>
     </row>
     <row r="70" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="43"/>
-      <c r="B70" s="52" t="s">
+      <c r="A70" s="51"/>
+      <c r="B70" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C70" s="44"/>
-      <c r="D70" s="45"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="53"/>
     </row>
     <row r="71" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="43"/>
-      <c r="B71" s="52" t="s">
+      <c r="A71" s="51"/>
+      <c r="B71" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C71" s="44"/>
-      <c r="D71" s="45"/>
+      <c r="C71" s="52"/>
+      <c r="D71" s="53"/>
     </row>
     <row r="72" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="3">
         <v>3</v>
       </c>
-      <c r="B72" s="53" t="s">
+      <c r="B72" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C72" s="44"/>
-      <c r="D72" s="45"/>
+      <c r="C72" s="52"/>
+      <c r="D72" s="53"/>
     </row>
     <row r="73" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="43">
+      <c r="A73" s="51">
         <v>3.1</v>
       </c>
-      <c r="B73" s="51" t="s">
+      <c r="B73" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C73" s="44"/>
-      <c r="D73" s="45"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="53"/>
     </row>
     <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="43"/>
-      <c r="B74" s="52" t="s">
+      <c r="A74" s="51"/>
+      <c r="B74" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="C74" s="44"/>
-      <c r="D74" s="45"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="53"/>
     </row>
     <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="43"/>
-      <c r="B75" s="52" t="s">
+      <c r="A75" s="51"/>
+      <c r="B75" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C75" s="44"/>
-      <c r="D75" s="45"/>
+      <c r="C75" s="52"/>
+      <c r="D75" s="53"/>
     </row>
     <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="43">
+      <c r="A76" s="51">
         <v>3.2</v>
       </c>
-      <c r="B76" s="51" t="s">
+      <c r="B76" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C76" s="44"/>
-      <c r="D76" s="45"/>
+      <c r="C76" s="52"/>
+      <c r="D76" s="53"/>
     </row>
     <row r="77" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="43"/>
-      <c r="B77" s="52" t="s">
+      <c r="A77" s="51"/>
+      <c r="B77" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C77" s="44"/>
-      <c r="D77" s="45"/>
+      <c r="C77" s="52"/>
+      <c r="D77" s="53"/>
     </row>
     <row r="78" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" s="43"/>
-      <c r="B78" s="52" t="s">
+      <c r="A78" s="51"/>
+      <c r="B78" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C78" s="44"/>
-      <c r="D78" s="45"/>
+      <c r="C78" s="52"/>
+      <c r="D78" s="53"/>
     </row>
     <row r="79" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="43">
+      <c r="A79" s="51">
         <v>3.3</v>
       </c>
-      <c r="B79" s="51" t="s">
+      <c r="B79" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C79" s="44"/>
-      <c r="D79" s="45"/>
+      <c r="C79" s="52"/>
+      <c r="D79" s="53"/>
     </row>
     <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="43"/>
-      <c r="B80" s="52" t="s">
+      <c r="A80" s="51"/>
+      <c r="B80" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C80" s="44"/>
-      <c r="D80" s="45"/>
+      <c r="C80" s="52"/>
+      <c r="D80" s="53"/>
     </row>
     <row r="81" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="43"/>
-      <c r="B81" s="52" t="s">
+      <c r="A81" s="51"/>
+      <c r="B81" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C81" s="44"/>
-      <c r="D81" s="45"/>
+      <c r="C81" s="52"/>
+      <c r="D81" s="53"/>
     </row>
     <row r="82" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="43">
+      <c r="A82" s="51">
         <v>3.4</v>
       </c>
-      <c r="B82" s="51" t="s">
+      <c r="B82" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C82" s="44"/>
-      <c r="D82" s="45"/>
+      <c r="C82" s="52"/>
+      <c r="D82" s="53"/>
     </row>
     <row r="83" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="43"/>
-      <c r="B83" s="52" t="s">
+      <c r="A83" s="51"/>
+      <c r="B83" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="C83" s="44"/>
-      <c r="D83" s="45"/>
+      <c r="C83" s="52"/>
+      <c r="D83" s="53"/>
     </row>
     <row r="84" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="43"/>
-      <c r="B84" s="5" t="s">
+      <c r="A84" s="51"/>
+      <c r="B84" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C84" s="44"/>
-      <c r="D84" s="45"/>
+      <c r="C84" s="52"/>
+      <c r="D84" s="53"/>
     </row>
     <row r="85" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="3">
@@ -2318,132 +2324,132 @@
       <c r="B85" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C85" s="44" t="s">
+      <c r="C85" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="D85" s="45">
+      <c r="D85" s="53">
         <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="43">
+      <c r="A86" s="51">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B86" s="51" t="s">
+      <c r="B86" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C86" s="44"/>
-      <c r="D86" s="45"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="53"/>
     </row>
     <row r="87" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="43"/>
-      <c r="B87" s="52" t="s">
+      <c r="A87" s="51"/>
+      <c r="B87" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C87" s="44"/>
-      <c r="D87" s="45"/>
+      <c r="C87" s="52"/>
+      <c r="D87" s="53"/>
     </row>
     <row r="88" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="43"/>
-      <c r="B88" s="52" t="s">
+      <c r="A88" s="51"/>
+      <c r="B88" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C88" s="44"/>
-      <c r="D88" s="45"/>
+      <c r="C88" s="52"/>
+      <c r="D88" s="53"/>
     </row>
     <row r="89" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="43"/>
-      <c r="B89" s="52" t="s">
+      <c r="A89" s="51"/>
+      <c r="B89" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C89" s="44"/>
-      <c r="D89" s="45"/>
+      <c r="C89" s="52"/>
+      <c r="D89" s="53"/>
     </row>
     <row r="90" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="43">
+      <c r="A90" s="51">
         <v>4.2</v>
       </c>
-      <c r="B90" s="51" t="s">
+      <c r="B90" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C90" s="44"/>
-      <c r="D90" s="45"/>
+      <c r="C90" s="52"/>
+      <c r="D90" s="53"/>
     </row>
     <row r="91" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="43"/>
-      <c r="B91" s="52" t="s">
+      <c r="A91" s="51"/>
+      <c r="B91" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C91" s="44"/>
-      <c r="D91" s="45"/>
+      <c r="C91" s="52"/>
+      <c r="D91" s="53"/>
     </row>
     <row r="92" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="43"/>
-      <c r="B92" s="52" t="s">
+      <c r="A92" s="51"/>
+      <c r="B92" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="C92" s="44"/>
-      <c r="D92" s="45"/>
+      <c r="C92" s="52"/>
+      <c r="D92" s="53"/>
     </row>
     <row r="93" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="43">
+      <c r="A93" s="51">
         <v>4.3</v>
       </c>
-      <c r="B93" s="51" t="s">
+      <c r="B93" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C93" s="44"/>
-      <c r="D93" s="45"/>
+      <c r="C93" s="52"/>
+      <c r="D93" s="53"/>
     </row>
     <row r="94" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="43"/>
-      <c r="B94" s="52" t="s">
+      <c r="A94" s="51"/>
+      <c r="B94" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="C94" s="44"/>
-      <c r="D94" s="45"/>
+      <c r="C94" s="52"/>
+      <c r="D94" s="53"/>
     </row>
     <row r="95" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="43"/>
-      <c r="B95" s="52" t="s">
+      <c r="A95" s="51"/>
+      <c r="B95" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C95" s="44"/>
-      <c r="D95" s="45"/>
+      <c r="C95" s="52"/>
+      <c r="D95" s="53"/>
     </row>
     <row r="96" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="43">
+      <c r="A96" s="51">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="C96" s="44"/>
-      <c r="D96" s="45"/>
+      <c r="C96" s="52"/>
+      <c r="D96" s="53"/>
     </row>
     <row r="97" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="43"/>
-      <c r="B97" s="5" t="s">
+      <c r="A97" s="51"/>
+      <c r="B97" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="C97" s="44"/>
-      <c r="D97" s="45"/>
+      <c r="C97" s="52"/>
+      <c r="D97" s="53"/>
     </row>
     <row r="98" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="43"/>
-      <c r="B98" s="5" t="s">
+      <c r="A98" s="51"/>
+      <c r="B98" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="C98" s="44"/>
-      <c r="D98" s="45"/>
+      <c r="C98" s="52"/>
+      <c r="D98" s="53"/>
     </row>
     <row r="99" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="43"/>
-      <c r="B99" s="5" t="s">
+      <c r="A99" s="51"/>
+      <c r="B99" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C99" s="44"/>
-      <c r="D99" s="45"/>
+      <c r="C99" s="52"/>
+      <c r="D99" s="53"/>
     </row>
     <row r="100" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="3">
@@ -2452,112 +2458,112 @@
       <c r="B100" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C100" s="44"/>
-      <c r="D100" s="45"/>
+      <c r="C100" s="52"/>
+      <c r="D100" s="53"/>
     </row>
     <row r="101" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="43">
+      <c r="A101" s="51">
         <v>5.0999999999999996</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C101" s="44"/>
-      <c r="D101" s="45"/>
+      <c r="C101" s="52"/>
+      <c r="D101" s="53"/>
     </row>
     <row r="102" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="43"/>
-      <c r="B102" s="5" t="s">
+      <c r="A102" s="51"/>
+      <c r="B102" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="C102" s="44"/>
-      <c r="D102" s="45"/>
+      <c r="C102" s="52"/>
+      <c r="D102" s="53"/>
     </row>
     <row r="103" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="43"/>
+      <c r="A103" s="51"/>
       <c r="B103" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C103" s="44"/>
-      <c r="D103" s="45"/>
+      <c r="C103" s="52"/>
+      <c r="D103" s="53"/>
     </row>
     <row r="104" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="43">
+      <c r="A104" s="51">
         <v>5.2</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C104" s="44"/>
-      <c r="D104" s="45"/>
+      <c r="C104" s="52"/>
+      <c r="D104" s="53"/>
     </row>
     <row r="105" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="43"/>
-      <c r="B105" s="5" t="s">
+      <c r="A105" s="51"/>
+      <c r="B105" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="44"/>
-      <c r="D105" s="45"/>
+      <c r="C105" s="52"/>
+      <c r="D105" s="53"/>
     </row>
     <row r="106" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="43"/>
-      <c r="B106" s="5" t="s">
+      <c r="A106" s="51"/>
+      <c r="B106" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C106" s="44"/>
-      <c r="D106" s="45"/>
+      <c r="C106" s="52"/>
+      <c r="D106" s="53"/>
     </row>
     <row r="107" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="43">
+      <c r="A107" s="51">
         <v>5.3</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C107" s="44"/>
-      <c r="D107" s="45"/>
+      <c r="C107" s="52"/>
+      <c r="D107" s="53"/>
     </row>
     <row r="108" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="43"/>
+      <c r="A108" s="51"/>
       <c r="B108" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C108" s="44"/>
-      <c r="D108" s="45"/>
+      <c r="C108" s="52"/>
+      <c r="D108" s="53"/>
     </row>
     <row r="109" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="43"/>
+      <c r="A109" s="51"/>
       <c r="B109" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C109" s="44"/>
-      <c r="D109" s="45"/>
+      <c r="C109" s="52"/>
+      <c r="D109" s="53"/>
     </row>
     <row r="110" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="43">
+      <c r="A110" s="51">
         <v>5.4</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C110" s="44"/>
-      <c r="D110" s="45"/>
+      <c r="C110" s="52"/>
+      <c r="D110" s="53"/>
     </row>
     <row r="111" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="43"/>
+      <c r="A111" s="51"/>
       <c r="B111" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C111" s="44"/>
-      <c r="D111" s="45"/>
+      <c r="C111" s="52"/>
+      <c r="D111" s="53"/>
     </row>
     <row r="112" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" s="43"/>
+      <c r="A112" s="51"/>
       <c r="B112" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C112" s="44"/>
-      <c r="D112" s="45"/>
+      <c r="C112" s="52"/>
+      <c r="D112" s="53"/>
     </row>
     <row r="113" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="3">
@@ -2566,296 +2572,296 @@
       <c r="B113" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C113" s="44"/>
-      <c r="D113" s="45"/>
+      <c r="C113" s="52"/>
+      <c r="D113" s="53"/>
     </row>
     <row r="114" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="46">
+      <c r="A114" s="54">
         <v>6.1</v>
       </c>
-      <c r="B114" s="51" t="s">
+      <c r="B114" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="C114" s="44"/>
-      <c r="D114" s="45"/>
+      <c r="C114" s="52"/>
+      <c r="D114" s="53"/>
     </row>
     <row r="115" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="46"/>
-      <c r="B115" s="52" t="s">
+      <c r="A115" s="54"/>
+      <c r="B115" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C115" s="44"/>
-      <c r="D115" s="45"/>
+      <c r="C115" s="52"/>
+      <c r="D115" s="53"/>
     </row>
     <row r="116" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="46"/>
-      <c r="B116" s="52" t="s">
+      <c r="A116" s="54"/>
+      <c r="B116" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C116" s="44"/>
-      <c r="D116" s="45"/>
+      <c r="C116" s="52"/>
+      <c r="D116" s="53"/>
     </row>
     <row r="117" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="46"/>
-      <c r="B117" s="52" t="s">
+      <c r="A117" s="54"/>
+      <c r="B117" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C117" s="44"/>
-      <c r="D117" s="45"/>
+      <c r="C117" s="52"/>
+      <c r="D117" s="53"/>
     </row>
     <row r="118" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="46"/>
-      <c r="B118" s="52" t="s">
+      <c r="A118" s="54"/>
+      <c r="B118" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="C118" s="44"/>
-      <c r="D118" s="45"/>
+      <c r="C118" s="52"/>
+      <c r="D118" s="53"/>
     </row>
     <row r="119" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="43">
+      <c r="A119" s="51">
         <v>6.2</v>
       </c>
-      <c r="B119" s="51" t="s">
+      <c r="B119" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C119" s="44"/>
-      <c r="D119" s="45"/>
+      <c r="C119" s="52"/>
+      <c r="D119" s="53"/>
     </row>
     <row r="120" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="43"/>
-      <c r="B120" s="52" t="s">
+      <c r="A120" s="51"/>
+      <c r="B120" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C120" s="44"/>
-      <c r="D120" s="45"/>
+      <c r="C120" s="52"/>
+      <c r="D120" s="53"/>
     </row>
     <row r="121" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="43"/>
-      <c r="B121" s="52" t="s">
+      <c r="A121" s="51"/>
+      <c r="B121" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="C121" s="44"/>
-      <c r="D121" s="45"/>
+      <c r="C121" s="52"/>
+      <c r="D121" s="53"/>
     </row>
     <row r="122" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="43"/>
-      <c r="B122" s="52" t="s">
+      <c r="A122" s="51"/>
+      <c r="B122" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="C122" s="44"/>
-      <c r="D122" s="45"/>
+      <c r="C122" s="52"/>
+      <c r="D122" s="53"/>
     </row>
     <row r="123" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="43"/>
-      <c r="B123" s="5" t="s">
+      <c r="A123" s="51"/>
+      <c r="B123" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="C123" s="44"/>
-      <c r="D123" s="45"/>
+      <c r="C123" s="52"/>
+      <c r="D123" s="53"/>
     </row>
     <row r="124" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="43">
+      <c r="A124" s="51">
         <v>6.3</v>
       </c>
-      <c r="B124" s="51" t="s">
+      <c r="B124" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C124" s="44"/>
-      <c r="D124" s="45"/>
+      <c r="C124" s="52"/>
+      <c r="D124" s="53"/>
     </row>
     <row r="125" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="43"/>
-      <c r="B125" s="52" t="s">
+      <c r="A125" s="51"/>
+      <c r="B125" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C125" s="44"/>
-      <c r="D125" s="45"/>
+      <c r="C125" s="52"/>
+      <c r="D125" s="53"/>
     </row>
     <row r="126" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126" s="43"/>
-      <c r="B126" s="52" t="s">
+      <c r="A126" s="51"/>
+      <c r="B126" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="C126" s="44"/>
-      <c r="D126" s="45"/>
+      <c r="C126" s="52"/>
+      <c r="D126" s="53"/>
     </row>
     <row r="127" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" s="43">
+      <c r="A127" s="51">
         <v>6.4</v>
       </c>
-      <c r="B127" s="51" t="s">
+      <c r="B127" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C127" s="44"/>
-      <c r="D127" s="45"/>
+      <c r="C127" s="52"/>
+      <c r="D127" s="53"/>
     </row>
     <row r="128" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="43"/>
-      <c r="B128" s="52" t="s">
+      <c r="A128" s="51"/>
+      <c r="B128" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="C128" s="44"/>
-      <c r="D128" s="45"/>
+      <c r="C128" s="52"/>
+      <c r="D128" s="53"/>
     </row>
     <row r="129" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="43"/>
-      <c r="B129" s="52" t="s">
+      <c r="A129" s="51"/>
+      <c r="B129" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="C129" s="44"/>
-      <c r="D129" s="45"/>
+      <c r="C129" s="52"/>
+      <c r="D129" s="53"/>
     </row>
     <row r="130" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A130" s="43">
+      <c r="A130" s="51">
         <v>6.5</v>
       </c>
       <c r="B130" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C130" s="44"/>
-      <c r="D130" s="45"/>
+      <c r="C130" s="52"/>
+      <c r="D130" s="53"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="43"/>
+      <c r="A131" s="51"/>
       <c r="B131" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C131" s="44"/>
-      <c r="D131" s="45"/>
+      <c r="C131" s="52"/>
+      <c r="D131" s="53"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="43"/>
+      <c r="A132" s="51"/>
       <c r="B132" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C132" s="44"/>
-      <c r="D132" s="45"/>
+      <c r="C132" s="52"/>
+      <c r="D132" s="53"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="43"/>
+      <c r="A133" s="51"/>
       <c r="B133" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C133" s="44"/>
-      <c r="D133" s="45"/>
+      <c r="C133" s="52"/>
+      <c r="D133" s="53"/>
     </row>
     <row r="134" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="3">
         <v>7</v>
       </c>
-      <c r="B134" s="8" t="s">
+      <c r="B134" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="C134" s="48" t="s">
+      <c r="C134" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="D134" s="47">
+      <c r="D134" s="55">
         <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" s="43">
+      <c r="A135" s="51">
         <v>7.1</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="C135" s="48"/>
-      <c r="D135" s="47"/>
+      <c r="C135" s="56"/>
+      <c r="D135" s="55"/>
     </row>
     <row r="136" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="43"/>
-      <c r="B136" s="5" t="s">
+      <c r="A136" s="51"/>
+      <c r="B136" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="C136" s="48"/>
-      <c r="D136" s="47"/>
+      <c r="C136" s="56"/>
+      <c r="D136" s="55"/>
     </row>
     <row r="137" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="43"/>
-      <c r="B137" s="5" t="s">
+      <c r="A137" s="51"/>
+      <c r="B137" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="C137" s="48"/>
-      <c r="D137" s="47"/>
+      <c r="C137" s="56"/>
+      <c r="D137" s="55"/>
     </row>
     <row r="138" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="43">
+      <c r="A138" s="51">
         <v>7.2</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B138" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C138" s="48"/>
-      <c r="D138" s="47"/>
+      <c r="C138" s="56"/>
+      <c r="D138" s="55"/>
     </row>
     <row r="139" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="43"/>
-      <c r="B139" s="5" t="s">
+      <c r="A139" s="51"/>
+      <c r="B139" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="C139" s="48"/>
-      <c r="D139" s="47"/>
+      <c r="C139" s="56"/>
+      <c r="D139" s="55"/>
     </row>
     <row r="140" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="43"/>
-      <c r="B140" s="5" t="s">
+      <c r="A140" s="51"/>
+      <c r="B140" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="C140" s="48"/>
-      <c r="D140" s="47"/>
+      <c r="C140" s="56"/>
+      <c r="D140" s="55"/>
     </row>
     <row r="141" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" s="43">
+      <c r="A141" s="51">
         <v>7.3</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B141" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="C141" s="48"/>
-      <c r="D141" s="47"/>
+      <c r="C141" s="56"/>
+      <c r="D141" s="55"/>
     </row>
     <row r="142" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142" s="43"/>
-      <c r="B142" s="5" t="s">
+      <c r="A142" s="51"/>
+      <c r="B142" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="C142" s="48"/>
-      <c r="D142" s="47"/>
+      <c r="C142" s="56"/>
+      <c r="D142" s="55"/>
     </row>
     <row r="143" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143" s="43"/>
-      <c r="B143" s="5" t="s">
+      <c r="A143" s="51"/>
+      <c r="B143" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="C143" s="48"/>
-      <c r="D143" s="47"/>
+      <c r="C143" s="56"/>
+      <c r="D143" s="55"/>
     </row>
     <row r="144" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" s="43">
+      <c r="A144" s="51">
         <v>7.4</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B144" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="C144" s="48"/>
-      <c r="D144" s="47"/>
+      <c r="C144" s="56"/>
+      <c r="D144" s="55"/>
     </row>
     <row r="145" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" s="43"/>
-      <c r="B145" s="5" t="s">
+      <c r="A145" s="51"/>
+      <c r="B145" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="C145" s="48"/>
-      <c r="D145" s="47"/>
+      <c r="C145" s="56"/>
+      <c r="D145" s="55"/>
     </row>
     <row r="146" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" s="43"/>
-      <c r="B146" s="5" t="s">
+      <c r="A146" s="51"/>
+      <c r="B146" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="C146" s="48"/>
-      <c r="D146" s="47"/>
+      <c r="C146" s="56"/>
+      <c r="D146" s="55"/>
     </row>
     <row r="147" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="6">
@@ -2864,8 +2870,8 @@
       <c r="B147" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C147" s="48"/>
-      <c r="D147" s="47"/>
+      <c r="C147" s="56"/>
+      <c r="D147" s="55"/>
     </row>
     <row r="148" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A148" s="6">
@@ -2874,90 +2880,90 @@
       <c r="B148" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="C148" s="48"/>
-      <c r="D148" s="47"/>
+      <c r="C148" s="56"/>
+      <c r="D148" s="55"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A149" s="43">
+      <c r="A149" s="51">
         <v>8.1</v>
       </c>
-      <c r="B149" s="12" t="s">
+      <c r="B149" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="C149" s="48"/>
-      <c r="D149" s="47"/>
+      <c r="C149" s="56"/>
+      <c r="D149" s="55"/>
     </row>
     <row r="150" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A150" s="43"/>
-      <c r="B150" s="9" t="s">
+      <c r="A150" s="51"/>
+      <c r="B150" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="C150" s="48"/>
-      <c r="D150" s="47"/>
+      <c r="C150" s="56"/>
+      <c r="D150" s="55"/>
     </row>
     <row r="151" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A151" s="43"/>
-      <c r="B151" s="13" t="s">
+      <c r="A151" s="51"/>
+      <c r="B151" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="C151" s="48"/>
-      <c r="D151" s="47"/>
+      <c r="C151" s="56"/>
+      <c r="D151" s="55"/>
     </row>
     <row r="152" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A152" s="43"/>
-      <c r="B152" s="13" t="s">
+      <c r="A152" s="51"/>
+      <c r="B152" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="C152" s="48"/>
-      <c r="D152" s="47"/>
+      <c r="C152" s="56"/>
+      <c r="D152" s="55"/>
     </row>
     <row r="153" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A153" s="43"/>
-      <c r="B153" s="13" t="s">
+      <c r="A153" s="51"/>
+      <c r="B153" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="C153" s="48"/>
-      <c r="D153" s="47"/>
+      <c r="C153" s="56"/>
+      <c r="D153" s="55"/>
     </row>
     <row r="154" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A154" s="43"/>
-      <c r="B154" s="13" t="s">
+      <c r="A154" s="51"/>
+      <c r="B154" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C154" s="48"/>
-      <c r="D154" s="47"/>
+      <c r="C154" s="56"/>
+      <c r="D154" s="55"/>
     </row>
     <row r="155" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A155" s="43"/>
-      <c r="B155" s="13" t="s">
+      <c r="A155" s="51"/>
+      <c r="B155" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="C155" s="48"/>
-      <c r="D155" s="47"/>
+      <c r="C155" s="56"/>
+      <c r="D155" s="55"/>
     </row>
     <row r="156" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A156" s="43"/>
-      <c r="B156" s="13" t="s">
+      <c r="A156" s="51"/>
+      <c r="B156" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="C156" s="48"/>
-      <c r="D156" s="47"/>
+      <c r="C156" s="56"/>
+      <c r="D156" s="55"/>
     </row>
     <row r="157" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A157" s="43"/>
+      <c r="A157" s="51"/>
       <c r="B157" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C157" s="48"/>
-      <c r="D157" s="47"/>
+      <c r="C157" s="56"/>
+      <c r="D157" s="55"/>
     </row>
     <row r="158" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A158" s="43"/>
+      <c r="A158" s="51"/>
       <c r="B158" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C158" s="48"/>
-      <c r="D158" s="47"/>
+      <c r="C158" s="56"/>
+      <c r="D158" s="55"/>
     </row>
     <row r="159" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="3">
@@ -2966,168 +2972,168 @@
       <c r="B159" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C159" s="48" t="s">
+      <c r="C159" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="D159" s="47">
+      <c r="D159" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A160" s="46">
+      <c r="A160" s="54">
         <v>9.1</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C160" s="48"/>
-      <c r="D160" s="47"/>
+      <c r="C160" s="56"/>
+      <c r="D160" s="55"/>
     </row>
     <row r="161" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A161" s="46"/>
+      <c r="A161" s="54"/>
       <c r="B161" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C161" s="48"/>
-      <c r="D161" s="47"/>
+      <c r="C161" s="56"/>
+      <c r="D161" s="55"/>
     </row>
     <row r="162" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A162" s="46"/>
+      <c r="A162" s="54"/>
       <c r="B162" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C162" s="48"/>
-      <c r="D162" s="47"/>
+      <c r="C162" s="56"/>
+      <c r="D162" s="55"/>
     </row>
     <row r="163" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A163" s="46"/>
+      <c r="A163" s="54"/>
       <c r="B163" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C163" s="48"/>
-      <c r="D163" s="47"/>
+      <c r="C163" s="56"/>
+      <c r="D163" s="55"/>
     </row>
     <row r="164" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A164" s="46"/>
+      <c r="A164" s="54"/>
       <c r="B164" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C164" s="48"/>
-      <c r="D164" s="47"/>
+      <c r="C164" s="56"/>
+      <c r="D164" s="55"/>
     </row>
     <row r="165" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A165" s="43">
+      <c r="A165" s="51">
         <v>9.1999999999999993</v>
       </c>
       <c r="B165" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C165" s="48"/>
-      <c r="D165" s="47"/>
+      <c r="C165" s="56"/>
+      <c r="D165" s="55"/>
     </row>
     <row r="166" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A166" s="43"/>
+      <c r="A166" s="51"/>
       <c r="B166" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C166" s="48"/>
-      <c r="D166" s="47"/>
+      <c r="C166" s="56"/>
+      <c r="D166" s="55"/>
     </row>
     <row r="167" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A167" s="43"/>
+      <c r="A167" s="51"/>
       <c r="B167" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C167" s="48"/>
-      <c r="D167" s="47"/>
+      <c r="C167" s="56"/>
+      <c r="D167" s="55"/>
     </row>
     <row r="168" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A168" s="43"/>
+      <c r="A168" s="51"/>
       <c r="B168" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C168" s="48"/>
-      <c r="D168" s="47"/>
+      <c r="C168" s="56"/>
+      <c r="D168" s="55"/>
     </row>
     <row r="169" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A169" s="43">
+      <c r="A169" s="51">
         <v>9.3000000000000007</v>
       </c>
       <c r="B169" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C169" s="48"/>
-      <c r="D169" s="47"/>
+      <c r="C169" s="56"/>
+      <c r="D169" s="55"/>
     </row>
     <row r="170" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A170" s="43"/>
+      <c r="A170" s="51"/>
       <c r="B170" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C170" s="48"/>
-      <c r="D170" s="47"/>
+      <c r="C170" s="56"/>
+      <c r="D170" s="55"/>
     </row>
     <row r="171" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A171" s="43"/>
+      <c r="A171" s="51"/>
       <c r="B171" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C171" s="48"/>
-      <c r="D171" s="47"/>
+      <c r="C171" s="56"/>
+      <c r="D171" s="55"/>
     </row>
     <row r="172" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A172" s="43"/>
-      <c r="B172" s="5" t="s">
+      <c r="A172" s="51"/>
+      <c r="B172" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="C172" s="48"/>
-      <c r="D172" s="47"/>
+      <c r="C172" s="56"/>
+      <c r="D172" s="55"/>
     </row>
     <row r="173" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A173" s="43">
+      <c r="A173" s="51">
         <v>9.4</v>
       </c>
       <c r="B173" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C173" s="48"/>
-      <c r="D173" s="47"/>
+      <c r="C173" s="56"/>
+      <c r="D173" s="55"/>
     </row>
     <row r="174" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A174" s="43"/>
+      <c r="A174" s="51"/>
       <c r="B174" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C174" s="48"/>
-      <c r="D174" s="47"/>
+      <c r="C174" s="56"/>
+      <c r="D174" s="55"/>
     </row>
     <row r="175" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A175" s="43"/>
+      <c r="A175" s="51"/>
       <c r="B175" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C175" s="48"/>
-      <c r="D175" s="47"/>
+      <c r="C175" s="56"/>
+      <c r="D175" s="55"/>
     </row>
     <row r="176" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A176" s="43"/>
+      <c r="A176" s="51"/>
       <c r="B176" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C176" s="48"/>
-      <c r="D176" s="47"/>
+      <c r="C176" s="56"/>
+      <c r="D176" s="55"/>
     </row>
     <row r="177" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A177" s="3">
         <v>10</v>
       </c>
-      <c r="B177" s="14" t="s">
+      <c r="B177" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="C177" s="44" t="s">
+      <c r="C177" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="D177" s="47">
+      <c r="D177" s="55">
         <v>1.5</v>
       </c>
     </row>
@@ -3135,11 +3141,11 @@
       <c r="A178" s="6">
         <v>10.1</v>
       </c>
-      <c r="B178" s="15" t="s">
+      <c r="B178" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="C178" s="44"/>
-      <c r="D178" s="47"/>
+      <c r="C178" s="52"/>
+      <c r="D178" s="55"/>
     </row>
     <row r="179" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="3">
@@ -3148,170 +3154,170 @@
       <c r="B179" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="C179" s="48" t="s">
+      <c r="C179" s="56" t="s">
         <v>188</v>
       </c>
-      <c r="D179" s="47">
+      <c r="D179" s="55">
         <v>0.5</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A180" s="43">
+      <c r="A180" s="51">
         <v>11.1</v>
       </c>
       <c r="B180" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C180" s="49"/>
-      <c r="D180" s="47"/>
+      <c r="C180" s="57"/>
+      <c r="D180" s="55"/>
     </row>
     <row r="181" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A181" s="43"/>
+      <c r="A181" s="51"/>
       <c r="B181" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C181" s="49"/>
-      <c r="D181" s="47"/>
+      <c r="C181" s="57"/>
+      <c r="D181" s="55"/>
     </row>
     <row r="182" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A182" s="43"/>
+      <c r="A182" s="51"/>
       <c r="B182" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C182" s="49"/>
-      <c r="D182" s="47"/>
+      <c r="C182" s="57"/>
+      <c r="D182" s="55"/>
     </row>
     <row r="183" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A183" s="43">
+      <c r="A183" s="51">
         <v>11.2</v>
       </c>
       <c r="B183" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C183" s="49"/>
-      <c r="D183" s="47"/>
+      <c r="C183" s="57"/>
+      <c r="D183" s="55"/>
     </row>
     <row r="184" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A184" s="43"/>
+      <c r="A184" s="51"/>
       <c r="B184" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C184" s="49"/>
-      <c r="D184" s="47"/>
+      <c r="C184" s="57"/>
+      <c r="D184" s="55"/>
     </row>
     <row r="185" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A185" s="43"/>
+      <c r="A185" s="51"/>
       <c r="B185" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C185" s="49"/>
-      <c r="D185" s="47"/>
+      <c r="C185" s="57"/>
+      <c r="D185" s="55"/>
     </row>
     <row r="186" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A186" s="50">
+      <c r="A186" s="58">
         <v>11.3</v>
       </c>
       <c r="B186" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C186" s="49"/>
-      <c r="D186" s="47"/>
+      <c r="C186" s="57"/>
+      <c r="D186" s="55"/>
     </row>
     <row r="187" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A187" s="50"/>
+      <c r="A187" s="58"/>
       <c r="B187" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="C187" s="49"/>
-      <c r="D187" s="47"/>
+      <c r="C187" s="57"/>
+      <c r="D187" s="55"/>
     </row>
     <row r="188" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A188" s="50"/>
+      <c r="A188" s="58"/>
       <c r="B188" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C188" s="49"/>
-      <c r="D188" s="47"/>
+      <c r="C188" s="57"/>
+      <c r="D188" s="55"/>
     </row>
     <row r="189" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A189" s="50"/>
+      <c r="A189" s="58"/>
       <c r="B189" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C189" s="49"/>
-      <c r="D189" s="47"/>
+      <c r="C189" s="57"/>
+      <c r="D189" s="55"/>
     </row>
     <row r="190" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A190" s="50">
+      <c r="A190" s="58">
         <v>11.4</v>
       </c>
       <c r="B190" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C190" s="49"/>
-      <c r="D190" s="47"/>
+      <c r="C190" s="57"/>
+      <c r="D190" s="55"/>
     </row>
     <row r="191" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A191" s="50"/>
+      <c r="A191" s="58"/>
       <c r="B191" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C191" s="49"/>
-      <c r="D191" s="47"/>
+      <c r="C191" s="57"/>
+      <c r="D191" s="55"/>
     </row>
     <row r="192" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A192" s="50"/>
+      <c r="A192" s="58"/>
       <c r="B192" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C192" s="49"/>
-      <c r="D192" s="47"/>
+      <c r="C192" s="57"/>
+      <c r="D192" s="55"/>
     </row>
     <row r="193" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A193" s="50">
+      <c r="A193" s="58">
         <v>11.5</v>
       </c>
       <c r="B193" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C193" s="49"/>
-      <c r="D193" s="47"/>
+      <c r="C193" s="57"/>
+      <c r="D193" s="55"/>
     </row>
     <row r="194" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A194" s="50"/>
+      <c r="A194" s="58"/>
       <c r="B194" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C194" s="49"/>
-      <c r="D194" s="47"/>
+      <c r="C194" s="57"/>
+      <c r="D194" s="55"/>
     </row>
     <row r="195" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A195" s="50"/>
+      <c r="A195" s="58"/>
       <c r="B195" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C195" s="49"/>
-      <c r="D195" s="47"/>
+      <c r="C195" s="57"/>
+      <c r="D195" s="55"/>
     </row>
     <row r="196" spans="1:4" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A196" s="50"/>
+      <c r="A196" s="58"/>
       <c r="B196" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C196" s="49"/>
-      <c r="D196" s="47"/>
+      <c r="C196" s="57"/>
+      <c r="D196" s="55"/>
     </row>
     <row r="197" spans="1:4" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="2">
         <v>12</v>
       </c>
-      <c r="B197" s="29" t="s">
+      <c r="B197" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="C197" s="27" t="s">
+      <c r="C197" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="D197" s="28">
+      <c r="D197" s="26">
         <v>1</v>
       </c>
     </row>

</xml_diff>